<commit_message>
EPBDS-8247 Add test for incorrect match
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Actions_Returns_4.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Actions_Returns_4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="159">
   <si>
     <t>Inputs</t>
   </si>
@@ -434,13 +434,69 @@
   </si>
   <si>
     <t>StringRange s</t>
+  </si>
+  <si>
+    <t>String name, Integer age, Date dateOfBirth, Integer flag</t>
+  </si>
+  <si>
+    <t>new myDatype(age, name, dateOfBirth );</t>
+  </si>
+  <si>
+    <t>result2</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>Datatype myDatype</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>myField1</t>
+  </si>
+  <si>
+    <t>myString</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>myDate1</t>
+  </si>
+  <si>
+    <t>Test myRules14</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>_res_.myField1</t>
+  </si>
+  <si>
+    <t>test5</t>
+  </si>
+  <si>
+    <t>_res_.myString</t>
+  </si>
+  <si>
+    <t>_res_.myDate1</t>
+  </si>
+  <si>
+    <t>SmartRules myDatype myRules14(String name, Integer age, Date dateOfBirth, Integer flag)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -479,12 +535,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442" rgb="C0504D"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -569,11 +625,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -618,6 +694,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -630,27 +712,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,43 +1147,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M109"/>
+  <dimension ref="B2:N116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="G108" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N116" sqref="L116:N116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="2.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="5.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="28.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="20.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="20.7109375" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" style="1" width="20.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="1" width="18.85546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="14" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="20" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="46.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="F2" s="20" t="s">
+      <c r="D2" s="25"/>
+      <c r="F2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="22"/>
+      <c r="I2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C3" s="10" t="s">
@@ -1125,16 +1232,16 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="23" t="s">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C7" s="7" t="s">
@@ -1285,15 +1392,15 @@
       <c r="K12" s="27"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="F14" s="23" t="s">
+      <c r="D14" s="25"/>
+      <c r="F14" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C15" s="15" t="s">
@@ -1358,14 +1465,14 @@
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="F20" s="23" t="s">
+      <c r="D20" s="25"/>
+      <c r="F20" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="23"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.2">
@@ -1423,16 +1530,16 @@
       <c r="G24" s="10"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="F26" s="23" t="s">
+      <c r="D26" s="22"/>
+      <c r="F26" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C27" s="15" t="s">
@@ -1509,15 +1616,15 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="F32" s="23" t="s">
+      <c r="D32" s="25"/>
+      <c r="F32" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.15">
       <c r="C33" s="15" t="s">
@@ -1579,15 +1686,15 @@
       </c>
       <c r="H36" s="10"/>
     </row>
-    <row r="39" spans="3:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="21" t="s">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C39" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="22"/>
-      <c r="F39" s="20" t="s">
+      <c r="D39" s="24"/>
+      <c r="F39" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="23"/>
+      <c r="G39" s="25"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="16" t="s">
@@ -1645,17 +1752,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="3:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="21" t="s">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C45" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="22"/>
-      <c r="F45" s="20" t="s">
+      <c r="D45" s="24"/>
+      <c r="F45" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
       <c r="J45" s="10"/>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.2">
@@ -1751,14 +1858,14 @@
       </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D51" s="22"/>
-      <c r="F51" s="20" t="s">
+      <c r="D51" s="24"/>
+      <c r="F51" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="G51" s="23"/>
+      <c r="G51" s="25"/>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C52" s="16" t="s">
@@ -1787,6 +1894,10 @@
       <c r="G53" s="10" t="s">
         <v>71</v>
       </c>
+      <c r="I53" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="J53" s="39"/>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C54" s="8" t="s">
@@ -1801,6 +1912,12 @@
       <c r="G54" s="10">
         <v>3</v>
       </c>
+      <c r="I54" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="J54" s="31" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C55" s="8" t="s">
@@ -1815,16 +1932,30 @@
       <c r="G55" s="10">
         <v>6</v>
       </c>
+      <c r="I55" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="I56" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="J56" s="40" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="F58" s="21" t="s">
+      <c r="D58" s="24"/>
+      <c r="F58" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="G58" s="22"/>
+      <c r="G58" s="24"/>
     </row>
     <row r="59" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C59" s="16" t="s">
@@ -1888,17 +2019,17 @@
       <c r="F63" s="12"/>
       <c r="G63" s="13"/>
     </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C65" s="21" t="s">
+    <row r="65" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C65" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="22"/>
-      <c r="F65" s="21" t="s">
+      <c r="D65" s="24"/>
+      <c r="F65" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="G65" s="22"/>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="G65" s="24"/>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C66" s="16" t="s">
         <v>127</v>
       </c>
@@ -1912,7 +2043,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C67" s="8" t="s">
         <v>128</v>
       </c>
@@ -1926,7 +2057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C68" s="8" t="s">
         <v>129</v>
       </c>
@@ -1940,7 +2071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C69" s="8" t="s">
         <v>130</v>
       </c>
@@ -1954,7 +2085,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C70" s="8" t="s">
         <v>131</v>
       </c>
@@ -1962,78 +2093,85 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="29"/>
-      <c r="D71" s="30"/>
-    </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C72" s="29"/>
-      <c r="D72" s="30"/>
-    </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C73" s="29"/>
-      <c r="D73" s="30"/>
-    </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C74" s="21" t="s">
+    <row r="71" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C71" s="20"/>
+      <c r="D71" s="21"/>
+    </row>
+    <row r="72" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C72" s="20"/>
+      <c r="D72" s="21"/>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C73" s="20"/>
+      <c r="D73" s="21"/>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C74" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="28"/>
-      <c r="K74" s="22"/>
-    </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="36"/>
+      <c r="J74" s="36"/>
+      <c r="K74" s="36"/>
+      <c r="L74" s="36"/>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C75" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D75" s="20" t="s">
+      <c r="D75" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20" t="s">
+      <c r="E75" s="22"/>
+      <c r="F75" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G75" s="20"/>
-      <c r="H75" s="20" t="s">
+      <c r="G75" s="22"/>
+      <c r="H75" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I75" s="20"/>
+      <c r="I75" s="22"/>
       <c r="J75" s="8" t="s">
         <v>34</v>
       </c>
       <c r="K75" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="76" spans="3:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L75" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="3:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="C76" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D76" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20" t="s">
+      <c r="E76" s="22"/>
+      <c r="F76" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="G76" s="20"/>
-      <c r="H76" s="20" t="s">
+      <c r="G76" s="22"/>
+      <c r="H76" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="I76" s="20"/>
+      <c r="I76" s="22"/>
       <c r="J76" s="8" t="s">
         <v>111</v>
       </c>
       <c r="K76" s="8" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L76" s="32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C77" s="18" t="s">
         <v>2</v>
       </c>
@@ -2043,49 +2181,55 @@
       <c r="E77" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F77" s="20" t="s">
+      <c r="F77" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G77" s="20"/>
-      <c r="H77" s="20" t="s">
+      <c r="G77" s="22"/>
+      <c r="H77" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="I77" s="20"/>
+      <c r="I77" s="22"/>
       <c r="J77" s="10" t="s">
         <v>35</v>
       </c>
       <c r="K77" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L77" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C78" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="24" t="s">
+      <c r="D78" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24" t="s">
+      <c r="E78" s="29"/>
+      <c r="F78" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24" t="s">
+      <c r="G78" s="29"/>
+      <c r="H78" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="I78" s="24"/>
+      <c r="I78" s="29"/>
       <c r="J78" s="14" t="s">
         <v>33</v>
       </c>
       <c r="K78" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-    </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L78" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+    </row>
+    <row r="80" spans="3:12" x14ac:dyDescent="0.2">
       <c r="D80" s="26" t="s">
         <v>95</v>
       </c>
@@ -2105,18 +2249,18 @@
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C82" s="20" t="s">
+    <row r="82" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C82" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="H82" s="20" t="s">
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="H82" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="I82" s="20"/>
-      <c r="J82" s="20"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="22"/>
     </row>
     <row r="83" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C83" s="8" t="s">
@@ -2125,10 +2269,10 @@
       <c r="D83" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="24" t="s">
+      <c r="E83" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="F83" s="24"/>
+      <c r="F83" s="29"/>
       <c r="H83" s="10" t="s">
         <v>8</v>
       </c>
@@ -2199,17 +2343,17 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="3:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C88" s="20" t="s">
+    <row r="88" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C88" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D88" s="20"/>
-      <c r="H88" s="20" t="s">
+      <c r="D88" s="22"/>
+      <c r="H88" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="I88" s="20"/>
-      <c r="J88" s="20"/>
-      <c r="K88" s="20"/>
+      <c r="I88" s="22"/>
+      <c r="J88" s="22"/>
+      <c r="K88" s="22"/>
       <c r="L88" s="10"/>
       <c r="M88" s="10"/>
     </row>
@@ -2329,19 +2473,19 @@
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C98" s="21" t="s">
+    <row r="98" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C98" s="23" t="s">
         <v>125</v>
       </c>
       <c r="D98" s="28"/>
-      <c r="E98" s="22"/>
-      <c r="H98" s="20" t="s">
+      <c r="E98" s="24"/>
+      <c r="H98" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="I98" s="20"/>
-      <c r="J98" s="20"/>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
+    </row>
+    <row r="99" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C99" s="8" t="s">
         <v>8</v>
       </c>
@@ -2361,7 +2505,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C100" s="10">
         <v>7</v>
       </c>
@@ -2381,7 +2525,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C101" s="10" t="s">
         <v>39</v>
       </c>
@@ -2401,7 +2545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H102" s="10">
         <v>6</v>
       </c>
@@ -2410,20 +2554,20 @@
       </c>
       <c r="J102" s="8"/>
     </row>
-    <row r="105" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C105" s="20" t="s">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C105" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D105" s="20"/>
-      <c r="E105" s="20"/>
-      <c r="H105" s="20" t="s">
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="H105" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="I105" s="20"/>
-      <c r="J105" s="20"/>
-      <c r="K105" s="20"/>
-    </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I105" s="28"/>
+      <c r="J105" s="28"/>
+      <c r="K105" s="24"/>
+    </row>
+    <row r="106" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
       <c r="C106" s="8" t="s">
         <v>8</v>
@@ -2447,7 +2591,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C107" s="10">
         <v>7</v>
       </c>
@@ -2470,7 +2614,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C108" s="10">
         <v>6</v>
       </c>
@@ -2493,7 +2637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H109" s="10">
         <v>6</v>
       </c>
@@ -2507,23 +2651,153 @@
         <v>8</v>
       </c>
     </row>
+    <row r="112" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C112" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="D112" s="38"/>
+      <c r="H112" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="I112" s="43"/>
+      <c r="J112" s="43"/>
+      <c r="K112" s="43"/>
+      <c r="L112" s="43"/>
+      <c r="M112" s="43"/>
+      <c r="N112" s="43"/>
+    </row>
+    <row r="113" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C113" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="D113" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="H113" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I113" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J113" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K113" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L113" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="N113" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C114" s="33">
+        <v>1</v>
+      </c>
+      <c r="D114" s="31">
+        <v>1</v>
+      </c>
+      <c r="H114" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I114" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="J114" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K114" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L114" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="M114" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="N114" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="115" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C115" s="33">
+        <v>2</v>
+      </c>
+      <c r="D115" s="31">
+        <v>2</v>
+      </c>
+      <c r="H115" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I115" s="10">
+        <v>4</v>
+      </c>
+      <c r="J115" s="41">
+        <v>43466</v>
+      </c>
+      <c r="K115" s="8">
+        <v>1</v>
+      </c>
+      <c r="L115" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M115" s="10">
+        <v>4</v>
+      </c>
+      <c r="N115" s="41">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="116" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C116" s="33">
+        <v>3</v>
+      </c>
+      <c r="D116" s="31">
+        <v>3</v>
+      </c>
+      <c r="H116" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="I116" s="10">
+        <v>2</v>
+      </c>
+      <c r="J116" s="41">
+        <v>43527</v>
+      </c>
+      <c r="K116" s="8">
+        <v>8</v>
+      </c>
+      <c r="L116" s="10"/>
+      <c r="M116" s="10"/>
+      <c r="N116" s="41"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="C82:F82"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C74:K74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D76:E76"/>
+  <mergeCells count="51">
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="H112:N112"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="H98:J98"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C74:L74"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="H78:I78"/>
+    <mergeCell ref="H82:J82"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F78:G78"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="F39:G39"/>
@@ -2540,23 +2814,21 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="H77:I77"/>
-    <mergeCell ref="H78:I78"/>
-    <mergeCell ref="H82:J82"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C82:F82"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D76:E76"/>
     <mergeCell ref="C88:D88"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="H98:J98"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="C98:E98"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
EPBDS-8247 Add test for External Condition + Smart Lookup
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Actions_Returns_4.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8247_Conditions_Actions_Returns_4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
   <si>
     <t>Inputs</t>
   </si>
@@ -491,6 +491,60 @@
   </si>
   <si>
     <t>SmartRules myDatype myRules14(String name, Integer age, Date dateOfBirth, Integer flag)</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>text3</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>SmartLookup Double mySmLookup2(alenaType d, Integer bla, Boolean val, String C)</t>
+  </si>
+  <si>
+    <t>d.a</t>
+  </si>
+  <si>
+    <t>d.b</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>Test mySmLookup2</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -649,7 +703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -700,63 +754,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N116"/>
+  <dimension ref="B2:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G108" zoomScale="125" workbookViewId="0">
-      <selection activeCell="N116" sqref="L116:N116"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1172,19 +1241,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="F2" s="22" t="s">
+      <c r="D2" s="33"/>
+      <c r="F2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="I2" s="25" t="s">
+      <c r="G2" s="32"/>
+      <c r="I2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C3" s="10" t="s">
@@ -1233,15 +1302,15 @@
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.15">
       <c r="C7" s="7" t="s">
@@ -1386,21 +1455,21 @@
       <c r="I12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="K12" s="27"/>
+      <c r="K12" s="35"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="F14" s="25" t="s">
+      <c r="D14" s="33"/>
+      <c r="F14" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C15" s="15" t="s">
@@ -1465,14 +1534,14 @@
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="F20" s="25" t="s">
+      <c r="D20" s="33"/>
+      <c r="F20" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="25"/>
+      <c r="G20" s="33"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.2">
@@ -1530,16 +1599,16 @@
       <c r="G24" s="10"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="F26" s="25" t="s">
+      <c r="D26" s="32"/>
+      <c r="F26" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C27" s="15" t="s">
@@ -1616,15 +1685,15 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="F32" s="25" t="s">
+      <c r="D32" s="33"/>
+      <c r="F32" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.15">
       <c r="C33" s="15" t="s">
@@ -1687,14 +1756,14 @@
       <c r="H36" s="10"/>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="24"/>
-      <c r="F39" s="22" t="s">
+      <c r="D39" s="31"/>
+      <c r="F39" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="G39" s="25"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="16" t="s">
@@ -1753,16 +1822,16 @@
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="24"/>
-      <c r="F45" s="22" t="s">
+      <c r="D45" s="31"/>
+      <c r="F45" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
       <c r="J45" s="10"/>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.2">
@@ -1858,14 +1927,14 @@
       </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="F51" s="22" t="s">
+      <c r="D51" s="31"/>
+      <c r="F51" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="G51" s="25"/>
+      <c r="G51" s="33"/>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C52" s="16" t="s">
@@ -1912,10 +1981,10 @@
       <c r="G54" s="10">
         <v>3</v>
       </c>
-      <c r="I54" s="33" t="s">
+      <c r="I54" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="J54" s="31" t="s">
+      <c r="J54" s="22" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1932,30 +2001,30 @@
       <c r="G55" s="10">
         <v>6</v>
       </c>
-      <c r="I55" s="33" t="s">
+      <c r="I55" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J55" s="31" t="s">
+      <c r="J55" s="22" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="56" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="I56" s="33" t="s">
+      <c r="I56" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="J56" s="40" t="s">
+      <c r="J56" s="26" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D58" s="24"/>
-      <c r="F58" s="23" t="s">
+      <c r="D58" s="31"/>
+      <c r="F58" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="G58" s="24"/>
+      <c r="G58" s="31"/>
     </row>
     <row r="59" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C59" s="16" t="s">
@@ -2020,14 +2089,14 @@
       <c r="G63" s="13"/>
     </row>
     <row r="65" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="24"/>
-      <c r="F65" s="23" t="s">
+      <c r="D65" s="31"/>
+      <c r="F65" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="G65" s="24"/>
+      <c r="G65" s="31"/>
     </row>
     <row r="66" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C66" s="16" t="s">
@@ -2106,42 +2175,42 @@
       <c r="D73" s="21"/>
     </row>
     <row r="74" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C74" s="35" t="s">
+      <c r="C74" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="36"/>
-      <c r="G74" s="36"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="36"/>
-      <c r="K74" s="36"/>
-      <c r="L74" s="36"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="45"/>
+      <c r="G74" s="45"/>
+      <c r="H74" s="45"/>
+      <c r="I74" s="45"/>
+      <c r="J74" s="45"/>
+      <c r="K74" s="45"/>
+      <c r="L74" s="45"/>
     </row>
     <row r="75" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C75" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D75" s="22" t="s">
+      <c r="D75" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E75" s="22"/>
-      <c r="F75" s="22" t="s">
+      <c r="E75" s="32"/>
+      <c r="F75" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G75" s="22"/>
-      <c r="H75" s="22" t="s">
+      <c r="G75" s="32"/>
+      <c r="H75" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="I75" s="22"/>
+      <c r="I75" s="32"/>
       <c r="J75" s="8" t="s">
         <v>34</v>
       </c>
       <c r="K75" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L75" s="31" t="s">
+      <c r="L75" s="22" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2149,25 +2218,25 @@
       <c r="C76" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D76" s="22" t="s">
+      <c r="D76" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22" t="s">
+      <c r="E76" s="32"/>
+      <c r="F76" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="G76" s="22"/>
-      <c r="H76" s="22" t="s">
+      <c r="G76" s="32"/>
+      <c r="H76" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I76" s="22"/>
+      <c r="I76" s="32"/>
       <c r="J76" s="8" t="s">
         <v>111</v>
       </c>
       <c r="K76" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="L76" s="32" t="s">
+      <c r="L76" s="23" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2181,21 +2250,21 @@
       <c r="E77" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F77" s="22" t="s">
+      <c r="F77" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="G77" s="22"/>
-      <c r="H77" s="22" t="s">
+      <c r="G77" s="32"/>
+      <c r="H77" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="I77" s="22"/>
+      <c r="I77" s="32"/>
       <c r="J77" s="10" t="s">
         <v>35</v>
       </c>
       <c r="K77" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="L77" s="33" t="s">
+      <c r="L77" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2203,45 +2272,45 @@
       <c r="C78" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="29" t="s">
+      <c r="D78" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E78" s="29"/>
-      <c r="F78" s="29" t="s">
+      <c r="E78" s="36"/>
+      <c r="F78" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29" t="s">
+      <c r="G78" s="36"/>
+      <c r="H78" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I78" s="29"/>
+      <c r="I78" s="36"/>
       <c r="J78" s="14" t="s">
         <v>33</v>
       </c>
       <c r="K78" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="L78" s="34" t="s">
+      <c r="L78" s="25" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="79" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D79" s="30"/>
-      <c r="E79" s="30"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
     </row>
     <row r="80" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="D80" s="26" t="s">
+      <c r="D80" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="26" t="s">
+      <c r="E80" s="35"/>
+      <c r="F80" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="G80" s="27"/>
-      <c r="H80" s="26" t="s">
+      <c r="G80" s="35"/>
+      <c r="H80" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="I80" s="27"/>
+      <c r="I80" s="35"/>
       <c r="J80" s="2" t="s">
         <v>61</v>
       </c>
@@ -2250,17 +2319,17 @@
       </c>
     </row>
     <row r="82" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C82" s="22" t="s">
+      <c r="C82" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D82" s="22"/>
-      <c r="E82" s="22"/>
-      <c r="F82" s="22"/>
-      <c r="H82" s="22" t="s">
+      <c r="D82" s="32"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="32"/>
+      <c r="H82" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="I82" s="22"/>
-      <c r="J82" s="22"/>
+      <c r="I82" s="32"/>
+      <c r="J82" s="32"/>
     </row>
     <row r="83" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C83" s="8" t="s">
@@ -2269,10 +2338,10 @@
       <c r="D83" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="29" t="s">
+      <c r="E83" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="F83" s="29"/>
+      <c r="F83" s="36"/>
       <c r="H83" s="10" t="s">
         <v>8</v>
       </c>
@@ -2344,16 +2413,16 @@
       </c>
     </row>
     <row r="88" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C88" s="22" t="s">
+      <c r="C88" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="D88" s="22"/>
-      <c r="H88" s="22" t="s">
+      <c r="D88" s="32"/>
+      <c r="H88" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I88" s="22"/>
-      <c r="J88" s="22"/>
-      <c r="K88" s="22"/>
+      <c r="I88" s="32"/>
+      <c r="J88" s="32"/>
+      <c r="K88" s="32"/>
       <c r="L88" s="10"/>
       <c r="M88" s="10"/>
     </row>
@@ -2474,16 +2543,16 @@
       </c>
     </row>
     <row r="98" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C98" s="23" t="s">
+      <c r="C98" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="D98" s="28"/>
-      <c r="E98" s="24"/>
-      <c r="H98" s="22" t="s">
+      <c r="D98" s="43"/>
+      <c r="E98" s="31"/>
+      <c r="H98" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="I98" s="22"/>
-      <c r="J98" s="22"/>
+      <c r="I98" s="32"/>
+      <c r="J98" s="32"/>
     </row>
     <row r="99" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C99" s="8" t="s">
@@ -2555,17 +2624,17 @@
       <c r="J102" s="8"/>
     </row>
     <row r="105" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C105" s="22" t="s">
+      <c r="C105" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="D105" s="22"/>
-      <c r="E105" s="22"/>
-      <c r="H105" s="23" t="s">
+      <c r="D105" s="32"/>
+      <c r="E105" s="32"/>
+      <c r="H105" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
-      <c r="K105" s="24"/>
+      <c r="I105" s="43"/>
+      <c r="J105" s="43"/>
+      <c r="K105" s="31"/>
     </row>
     <row r="106" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
@@ -2656,21 +2725,21 @@
         <v>158</v>
       </c>
       <c r="D112" s="38"/>
-      <c r="H112" s="42" t="s">
+      <c r="H112" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="I112" s="43"/>
-      <c r="J112" s="43"/>
-      <c r="K112" s="43"/>
-      <c r="L112" s="43"/>
-      <c r="M112" s="43"/>
-      <c r="N112" s="43"/>
+      <c r="I112" s="41"/>
+      <c r="J112" s="41"/>
+      <c r="K112" s="41"/>
+      <c r="L112" s="41"/>
+      <c r="M112" s="41"/>
+      <c r="N112" s="41"/>
     </row>
     <row r="113" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C113" s="31" t="s">
+      <c r="C113" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D113" s="44" t="s">
+      <c r="D113" s="28" t="s">
         <v>142</v>
       </c>
       <c r="H113" s="10" t="s">
@@ -2696,10 +2765,10 @@
       </c>
     </row>
     <row r="114" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C114" s="33">
+      <c r="C114" s="24">
         <v>1</v>
       </c>
-      <c r="D114" s="31">
+      <c r="D114" s="22">
         <v>1</v>
       </c>
       <c r="H114" s="10" t="s">
@@ -2725,10 +2794,10 @@
       </c>
     </row>
     <row r="115" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C115" s="33">
+      <c r="C115" s="24">
         <v>2</v>
       </c>
-      <c r="D115" s="31">
+      <c r="D115" s="22">
         <v>2</v>
       </c>
       <c r="H115" s="10" t="s">
@@ -2737,7 +2806,7 @@
       <c r="I115" s="10">
         <v>4</v>
       </c>
-      <c r="J115" s="41">
+      <c r="J115" s="27">
         <v>43466</v>
       </c>
       <c r="K115" s="8">
@@ -2749,15 +2818,15 @@
       <c r="M115" s="10">
         <v>4</v>
       </c>
-      <c r="N115" s="41">
+      <c r="N115" s="27">
         <v>43466</v>
       </c>
     </row>
     <row r="116" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C116" s="33">
+      <c r="C116" s="24">
         <v>3</v>
       </c>
-      <c r="D116" s="31">
+      <c r="D116" s="22">
         <v>3</v>
       </c>
       <c r="H116" s="10" t="s">
@@ -2766,7 +2835,7 @@
       <c r="I116" s="10">
         <v>2</v>
       </c>
-      <c r="J116" s="41">
+      <c r="J116" s="27">
         <v>43527</v>
       </c>
       <c r="K116" s="8">
@@ -2774,12 +2843,177 @@
       </c>
       <c r="L116" s="10"/>
       <c r="M116" s="10"/>
-      <c r="N116" s="41"/>
+      <c r="N116" s="27"/>
+    </row>
+    <row r="121" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C121" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29"/>
+      <c r="F121" s="29"/>
+      <c r="G121" s="29"/>
+    </row>
+    <row r="122" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C122" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E122" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="F122" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="G122" s="49" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="123" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C123" s="10">
+        <v>100</v>
+      </c>
+      <c r="D123" s="10">
+        <v>100</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F123" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="G123" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="124" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C124" s="10">
+        <v>200</v>
+      </c>
+      <c r="D124" s="10">
+        <v>200</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="F124" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="G124" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="125" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C125" s="10">
+        <v>300</v>
+      </c>
+      <c r="D125" s="10">
+        <v>300</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F125" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G125" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C129" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="D129" s="47"/>
+      <c r="E129" s="47"/>
+      <c r="F129" s="47"/>
+      <c r="G129" s="47"/>
+      <c r="H129" s="47"/>
+    </row>
+    <row r="130" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C130" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D130" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E130" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F130" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G130" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H130" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="131" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C131" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D131" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E131" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F131" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G131" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H131" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C132" s="10">
+        <v>100</v>
+      </c>
+      <c r="D132" s="10">
+        <v>100</v>
+      </c>
+      <c r="E132" s="10">
+        <v>100</v>
+      </c>
+      <c r="F132" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G132" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="H132" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C133" s="10">
+        <v>200</v>
+      </c>
+      <c r="D133" s="10">
+        <v>200</v>
+      </c>
+      <c r="E133" s="10">
+        <v>200</v>
+      </c>
+      <c r="F133" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G133" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="H133" s="10" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="51">
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="I53:J53"/>
+  <mergeCells count="53">
     <mergeCell ref="H112:N112"/>
     <mergeCell ref="H88:K88"/>
     <mergeCell ref="H98:J98"/>
@@ -2789,6 +3023,9 @@
     <mergeCell ref="D79:E79"/>
     <mergeCell ref="C98:E98"/>
     <mergeCell ref="C74:L74"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="C88:D88"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="H76:I76"/>
     <mergeCell ref="H77:I77"/>
@@ -2798,6 +3035,9 @@
     <mergeCell ref="F77:G77"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="F78:G78"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="H75:I75"/>
+    <mergeCell ref="I53:J53"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="F39:G39"/>
@@ -2814,21 +3054,19 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="C121:G121"/>
     <mergeCell ref="C51:D51"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="C82:F82"/>
     <mergeCell ref="D80:E80"/>
     <mergeCell ref="F80:G80"/>
-    <mergeCell ref="H80:I80"/>
     <mergeCell ref="C58:D58"/>
     <mergeCell ref="D75:E75"/>
     <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
     <mergeCell ref="D78:E78"/>
     <mergeCell ref="D76:E76"/>
-    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C129:H129"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>